<commit_message>
Edit file via upload
Removed reference to p-values or confidence intervals as z-scores from this analysis do not follow a normal distribution.
</commit_message>
<xml_diff>
--- a/excel_sheet_for_adjusting_1_voxel.xlsx
+++ b/excel_sheet_for_adjusting_1_voxel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Fixed and random" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="79">
   <si>
     <t>Estimate</t>
   </si>
@@ -51,22 +51,13 @@
     <t>Numerator</t>
   </si>
   <si>
-    <t>95% lower</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>95% upper</t>
-  </si>
-  <si>
     <t>Tau-sq</t>
   </si>
   <si>
     <t>Z</t>
-  </si>
-  <si>
-    <t>p 1 tailed</t>
   </si>
   <si>
     <t>Park_2017</t>
@@ -502,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -597,31 +588,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -636,6 +607,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -645,16 +646,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,38 +953,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="A2" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1000,77 +992,77 @@
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
       <c r="K2" s="61" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L2" s="61"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="60" t="s">
-        <v>57</v>
+      <c r="M2" s="62"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="69" t="s">
+        <v>54</v>
       </c>
       <c r="P2" s="61"/>
       <c r="Q2" s="61"/>
-      <c r="R2" s="62"/>
+      <c r="R2" s="63"/>
     </row>
     <row r="3" spans="1:18" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="28" t="s">
+      <c r="J3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="N3" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="28" t="s">
+      <c r="O3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="Q3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3" s="28" t="s">
+      <c r="R3" s="32" t="s">
         <v>53</v>
-      </c>
-      <c r="P3" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="32" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -1140,7 +1132,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="11">
         <v>0</v>
@@ -1210,7 +1202,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="11">
         <v>0.318718</v>
@@ -1280,7 +1272,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="11">
         <v>1.3027059999999999</v>
@@ -1350,7 +1342,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -1420,7 +1412,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="11">
         <v>0.12754799999999999</v>
@@ -1490,7 +1482,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" s="11">
         <v>0</v>
@@ -1560,7 +1552,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="11">
         <v>0.28117799999999998</v>
@@ -1630,7 +1622,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" s="11">
         <v>0</v>
@@ -1700,7 +1692,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="11">
         <v>0</v>
@@ -1770,7 +1762,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" s="11">
         <v>-1.7840000000000002E-2</v>
@@ -1840,7 +1832,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B15" s="11">
         <v>0.14366799999999999</v>
@@ -1910,7 +1902,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="11">
         <v>-8.1759999999999992E-3</v>
@@ -1980,7 +1972,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="11">
         <v>0.16692000000000001</v>
@@ -2050,7 +2042,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="11">
         <v>0</v>
@@ -2120,7 +2112,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" s="11">
         <v>0.23039399999999999</v>
@@ -2190,7 +2182,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="11">
         <v>0</v>
@@ -2260,7 +2252,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="11">
         <v>0.43754399999999999</v>
@@ -2330,13 +2322,13 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F22" s="23">
         <f>SUM(F4:F21)</f>
@@ -2355,7 +2347,7 @@
         <v>35125.754530206505</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
@@ -2368,7 +2360,7 @@
         <v>43.188414769725064</v>
       </c>
       <c r="O22" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P22" s="23"/>
       <c r="Q22" s="23">
@@ -2382,13 +2374,13 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="4"/>
       <c r="E23" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F23" s="21">
         <f>(SUMIF(B4:B21, "&lt;&gt; 0", F4:F21))+(SUMIFS(F4:F21, B4:B21, "= 0", D4:D21,"=0"))</f>
@@ -2441,57 +2433,57 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="58"/>
-      <c r="G25" s="59"/>
+      <c r="E25" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="62"/>
+      <c r="G25" s="68"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="54" t="s">
+      <c r="I25" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="J25" s="55"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="N25" s="59"/>
+      <c r="N25" s="68"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
-      <c r="Q25" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="R25" s="62"/>
+      <c r="Q25" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="R25" s="63"/>
     </row>
     <row r="26" spans="1:26" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="27"/>
       <c r="F26" s="43" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G26" s="43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="26"/>
       <c r="J26" s="43" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K26" s="43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M26" s="27"/>
       <c r="N26" s="52" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q26" s="51"/>
       <c r="R26" s="53" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="45">
         <f>COUNTA(B4:B21)</f>
@@ -2537,7 +2529,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B28" s="48">
         <f>COUNTIF(B4:B21, "&lt;&gt; 0")+(COUNTIFS(B4:B21, "= 0", D4:D21,"=0"))</f>
@@ -2622,26 +2614,26 @@
       <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="49">
-        <f>F27-1.96*F29</f>
-        <v>3.3271639348545726E-2</v>
-      </c>
-      <c r="G30" s="49">
-        <f>G27-1.96*G29</f>
-        <v>6.4671999824401541E-2</v>
+      <c r="A30" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="50">
+        <f>F27/F29</f>
+        <v>2.7605625056109888</v>
+      </c>
+      <c r="G30" s="50">
+        <f>G27/G29</f>
+        <v>3.2726207001646936</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J30" s="18">
         <f>F22-I22/F22</f>
@@ -2651,43 +2643,33 @@
         <f>F23-I23/F23</f>
         <v>335.5327336219994</v>
       </c>
-      <c r="M30" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="N30" s="18">
-        <f>N27-1.96*N29</f>
-        <v>2.4775935960940854E-2</v>
-      </c>
-      <c r="Q30" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="R30" s="18">
-        <f>R27-1.96*R29</f>
-        <v>6.465178359157106E-2</v>
+      <c r="M30" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="N30" s="20">
+        <f>N27/N29</f>
+        <v>2.4049327698489007</v>
+      </c>
+      <c r="Q30" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="R30" s="20">
+        <f>R27/R29</f>
+        <v>2.6966986498723235</v>
       </c>
       <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="49">
-        <f>F27+1.96*F29</f>
-        <v>0.19618812036305328</v>
-      </c>
-      <c r="G31" s="49">
-        <f>G27+1.96*G29</f>
-        <v>0.25780794479300201</v>
-      </c>
+      <c r="A31" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="8"/>
       <c r="H31" s="11"/>
       <c r="I31" s="36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J31" s="20">
         <f>J29/J30</f>
@@ -2697,72 +2679,10 @@
         <f>K29/K30</f>
         <v>4.2536671268532333E-2</v>
       </c>
-      <c r="M31" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="N31" s="18">
-        <f>N27+1.96*N29</f>
-        <v>0.24305985557394366</v>
-      </c>
-      <c r="Q31" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="R31" s="18">
-        <f>R27+1.96*R29</f>
-        <v>0.40866624828874565</v>
-      </c>
       <c r="Z31" s="11"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E32" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="50">
-        <f>F27/F29</f>
-        <v>2.7605625056109888</v>
-      </c>
-      <c r="G32" s="50">
-        <f>G27/G29</f>
-        <v>3.2726207001646936</v>
-      </c>
-      <c r="M32" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="N32" s="18">
-        <f>N27/N29</f>
-        <v>2.4049327698489007</v>
-      </c>
-      <c r="Q32" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="R32" s="18">
-        <f>R27/R29</f>
-        <v>2.6966986498723235</v>
-      </c>
-    </row>
-    <row r="33" spans="13:18" x14ac:dyDescent="0.25">
-      <c r="M33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N33" s="20">
-        <f>(1-(NORMDIST((N32),0,1,TRUE)))</f>
-        <v>8.0877206223504139E-3</v>
-      </c>
-      <c r="Q33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="R33" s="20">
-        <f>(1-(NORMDIST((R32),0,1,TRUE)))</f>
-        <v>3.5015306799573986E-3</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="I25:K25"/>
@@ -2770,6 +2690,11 @@
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2778,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA44"/>
+  <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2806,40 +2731,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64"/>
+      <c r="A2" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -2847,80 +2772,80 @@
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
       <c r="L2" s="61" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M2" s="61"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="60" t="s">
-        <v>57</v>
+      <c r="N2" s="62"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="69" t="s">
+        <v>54</v>
       </c>
       <c r="Q2" s="61"/>
       <c r="R2" s="61"/>
-      <c r="S2" s="62"/>
+      <c r="S2" s="63"/>
     </row>
     <row r="3" spans="1:27" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="28" t="s">
+      <c r="K3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="O3" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="28" t="s">
+      <c r="P3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="R3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="28" t="s">
+      <c r="S3" s="32" t="s">
         <v>53</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="32" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -2993,7 +2918,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="11">
         <v>0</v>
@@ -3066,7 +2991,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="11">
         <v>0.318718</v>
@@ -3139,7 +3064,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="11">
         <v>1.3027059999999999</v>
@@ -3212,7 +3137,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -3285,7 +3210,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="11">
         <v>0.12754799999999999</v>
@@ -3358,7 +3283,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" s="11">
         <v>0</v>
@@ -3431,7 +3356,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="11">
         <v>0.28117799999999998</v>
@@ -3504,7 +3429,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" s="11">
         <v>0</v>
@@ -3577,7 +3502,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="11">
         <v>0</v>
@@ -3656,7 +3581,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" s="11">
         <v>-1.7840000000000002E-2</v>
@@ -3729,7 +3654,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="11">
         <v>0.14366799999999999</v>
@@ -3802,7 +3727,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="11">
         <v>-8.1759999999999992E-3</v>
@@ -3875,7 +3800,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="11">
         <v>0.16692000000000001</v>
@@ -3948,7 +3873,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="11">
         <v>0</v>
@@ -4021,7 +3946,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" s="11">
         <v>0.23039399999999999</v>
@@ -4094,7 +4019,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="11">
         <v>0</v>
@@ -4167,7 +4092,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="11">
         <v>0.43754399999999999</v>
@@ -4240,7 +4165,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4287,7 +4212,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4322,7 +4247,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4369,7 +4294,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4437,15 +4362,15 @@
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
-      <c r="N27" s="60" t="s">
-        <v>39</v>
+      <c r="N27" s="69" t="s">
+        <v>36</v>
       </c>
       <c r="O27" s="61"/>
       <c r="P27" s="61"/>
       <c r="Q27" s="61"/>
       <c r="R27" s="61"/>
       <c r="S27" s="61"/>
-      <c r="T27" s="62"/>
+      <c r="T27" s="63"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -4453,69 +4378,69 @@
       <c r="C28" s="8"/>
       <c r="D28" s="15"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="60" t="s">
-        <v>38</v>
+      <c r="F28" s="69" t="s">
+        <v>35</v>
       </c>
       <c r="G28" s="61"/>
-      <c r="H28" s="62"/>
+      <c r="H28" s="63"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="68"/>
-      <c r="L28" s="69"/>
+      <c r="J28" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="72"/>
+      <c r="L28" s="73"/>
       <c r="M28" s="8"/>
       <c r="N28" s="35"/>
-      <c r="O28" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="S28" s="55"/>
-      <c r="T28" s="56"/>
+      <c r="O28" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="S28" s="65"/>
+      <c r="T28" s="66"/>
     </row>
     <row r="29" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F29" s="26"/>
       <c r="G29" s="43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H29" s="43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="26"/>
       <c r="K29" s="43" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L29" s="39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N29" s="27"/>
       <c r="O29" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="P29" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q29" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="P29" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q29" s="39" t="s">
-        <v>77</v>
-      </c>
       <c r="R29" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="S29" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="T29" s="39" t="s">
         <v>74</v>
-      </c>
-      <c r="S29" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="T29" s="39" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="46">
         <f>COUNTA(B4:B21)</f>
@@ -4574,7 +4499,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B31" s="47">
         <f>COUNTIF(B4:B21, "&lt;&gt; 0")+(COUNTIFS(B4:B21, "= 0", E4:E21,"=0"))</f>
@@ -4595,11 +4520,11 @@
       <c r="J31" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="K31" s="15">
+      <c r="K31" s="74">
         <f>COUNT(B4:B21)-2</f>
         <v>16</v>
       </c>
-      <c r="L31" s="18">
+      <c r="L31" s="47">
         <f>COUNTIF(B4:B21, "&lt;&gt; 0")+(COUNTIFS(B4:B21, "= 0", E4:E21,"=0"))-2</f>
         <v>8</v>
       </c>
@@ -4633,7 +4558,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B32" s="41">
         <f>COUNTIF(D4:D21, "=0")</f>
@@ -4692,26 +4617,26 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B33" s="41">
         <f>COUNTIF(D4:D21, "=1")</f>
         <v>9</v>
       </c>
-      <c r="F33" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="15">
-        <f>G30-1.96*G32</f>
-        <v>7.3875407664053677E-2</v>
-      </c>
-      <c r="H33" s="18">
-        <f>H30-1.96*H32</f>
-        <v>-5.0106155594026612E-2</v>
+      <c r="F33" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="21">
+        <f>G30/G32</f>
+        <v>3.0907066656844999</v>
+      </c>
+      <c r="H33" s="20">
+        <f>H30/H32</f>
+        <v>1.0297372765069495</v>
       </c>
       <c r="I33" s="11"/>
       <c r="J33" s="41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K33" s="15">
         <f>(G22-J22/G22) + (G24-J24/G24)</f>
@@ -4721,50 +4646,45 @@
         <f>(G23-J23/G23) + (G25-J25/G25)</f>
         <v>271.85936702981564</v>
       </c>
-      <c r="N33" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="O33" s="13">
-        <f>O30-1.96*O32</f>
-        <v>3.823220873253369E-2</v>
-      </c>
-      <c r="P33" s="15">
-        <f>P30-1.96*P32</f>
-        <v>-6.4043518217724013E-2</v>
-      </c>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="13">
-        <f>R30-1.96*R32</f>
-        <v>0.15460821662565088</v>
-      </c>
-      <c r="S33" s="15">
-        <f>S30-1.96*S32</f>
-        <v>-7.3394957731690288E-2</v>
-      </c>
-      <c r="T33" s="16"/>
+      <c r="N33" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="O33" s="19">
+        <f>O30/O32</f>
+        <v>2.433382655167124</v>
+      </c>
+      <c r="P33" s="21">
+        <f t="shared" ref="P33:Q33" si="13">P30/P32</f>
+        <v>1.0890668821041445</v>
+      </c>
+      <c r="Q33" s="22">
+        <f t="shared" si="13"/>
+        <v>-1.0661066888998465</v>
+      </c>
+      <c r="R33" s="19">
+        <f>R30/R32</f>
+        <v>3.1527770414765914</v>
+      </c>
+      <c r="S33" s="21">
+        <f>S30/S32</f>
+        <v>1.2154550248241682</v>
+      </c>
+      <c r="T33" s="22">
+        <f>T30/T32</f>
+        <v>-1.7737503629699143</v>
+      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B34" s="47">
         <f>COUNTIFS(B4:B21, "&lt;&gt; 0", D4:D21, "=0")+(COUNTIFS(B4:B21, "= 0", E4:E21,"=0", D4:D21, "=0"))</f>
         <v>4</v>
       </c>
-      <c r="F34" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="15">
-        <f>G30+1.96*G32</f>
-        <v>0.32999099168935819</v>
-      </c>
-      <c r="H34" s="18">
-        <f>H30+1.96*H32</f>
-        <v>0.16103433726702227</v>
-      </c>
       <c r="I34" s="11"/>
       <c r="J34" s="42" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K34" s="21">
         <f>K32/K33</f>
@@ -4774,208 +4694,96 @@
         <f>L32/L33</f>
         <v>2.853078604947085E-2</v>
       </c>
-      <c r="N34" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="O34" s="13">
-        <f>O30+1.96*O32</f>
-        <v>0.35482652539295612</v>
-      </c>
-      <c r="P34" s="15">
-        <f>P30+1.96*P32</f>
-        <v>0.22421121254737508</v>
-      </c>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="13">
-        <f>R30+1.96*R32</f>
-        <v>0.66272011692034294</v>
-      </c>
-      <c r="S34" s="15">
-        <f>S30+1.96*S32</f>
-        <v>0.31302660698343082</v>
-      </c>
-      <c r="T34" s="16"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="73">
+        <v>70</v>
+      </c>
+      <c r="B35" s="54">
         <f>COUNTIFS(B4:B21, "&lt;&gt; 0", D4:D21, "=1")+(COUNTIFS(B4:B21, "= 0", E4:E21,"=0", D4:D21, "=1"))</f>
         <v>6</v>
       </c>
-      <c r="F35" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="21">
-        <f>G30/G32</f>
-        <v>3.0907066656844999</v>
-      </c>
-      <c r="H35" s="20">
-        <f>H30/H32</f>
-        <v>1.0297372765069495</v>
-      </c>
-      <c r="N35" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="O35" s="13">
-        <f>O30/O32</f>
-        <v>2.433382655167124</v>
-      </c>
-      <c r="P35" s="15">
-        <f t="shared" ref="P35:Q35" si="13">P30/P32</f>
-        <v>1.0890668821041445</v>
-      </c>
-      <c r="Q35" s="16">
-        <f t="shared" si="13"/>
-        <v>-1.0661066888998465</v>
-      </c>
-      <c r="R35" s="13">
-        <f>R30/R32</f>
-        <v>3.1527770414765914</v>
-      </c>
-      <c r="S35" s="15">
-        <f>S30/S32</f>
-        <v>1.2154550248241682</v>
-      </c>
-      <c r="T35" s="16">
-        <f>T30/T32</f>
-        <v>-1.7737503629699143</v>
-      </c>
+      <c r="F35" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="61"/>
+      <c r="H35" s="63"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="O36" s="19">
-        <f>(1-(NORMDIST((O35),0,1,TRUE)))</f>
-        <v>7.4792415695529302E-3</v>
-      </c>
-      <c r="P36" s="21">
-        <f>(1-(NORMDIST((P35),0,1,TRUE)))</f>
-        <v>0.13806219648660756</v>
-      </c>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="21">
-        <f>(1-(NORMDIST((S35),0,1,TRUE)))</f>
-        <v>0.11209629620495298</v>
-      </c>
-      <c r="T36" s="22"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" s="43" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F37" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="G37" s="61"/>
-      <c r="H37" s="62"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="72"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="H38" s="43" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="72" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="F39" s="41" t="s">
+      <c r="F37" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G37" s="15">
         <f>H23/G23</f>
         <v>0.35766435931379104</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H37" s="18">
         <f>H25/G25</f>
         <v>6.8353961585657833E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F40" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="G40" s="15">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="F38" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="15">
         <f>1/G23</f>
         <v>7.560801125468382E-3</v>
       </c>
-      <c r="H40" s="18">
+      <c r="H38" s="18">
         <f>1/G25</f>
         <v>3.575384223532603E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F41" s="41" t="s">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="F39" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="15">
-        <f>SQRT(G40)</f>
+      <c r="G39" s="15">
+        <f>SQRT(G38)</f>
         <v>8.6952867264216083E-2</v>
       </c>
-      <c r="H41" s="18">
-        <f>SQRT(H40)</f>
+      <c r="H39" s="18">
+        <f>SQRT(H38)</f>
         <v>5.9794516667773169E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F42" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="15">
-        <f>G39-1.96*G41</f>
-        <v>0.1872367394759275</v>
-      </c>
-      <c r="H42" s="18">
-        <f>H39-1.96*H41</f>
-        <v>-4.8843291083177573E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F43" s="41" t="s">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F40" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="15">
-        <f>G39+1.96*G41</f>
-        <v>0.52809197915165451</v>
-      </c>
-      <c r="H43" s="18">
-        <f>H39+1.96*H41</f>
-        <v>0.18555121425449322</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F44" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="21">
-        <f>G39/G41</f>
+      <c r="G40" s="21">
+        <f>G37/G39</f>
         <v>4.1133130000990947</v>
       </c>
-      <c r="H44" s="20">
-        <f>H39/H41</f>
+      <c r="H40" s="20">
+        <f>H37/H39</f>
         <v>1.143147656254873</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="O28:Q28"/>
-    <mergeCell ref="R28:T28"/>
     <mergeCell ref="N27:T27"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="J28:L28"/>
@@ -4985,6 +4793,11 @@
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="P2:S2"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="O28:Q28"/>
+    <mergeCell ref="R28:T28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>